<commit_message>
Fix ranking. Use 'rankdata' instead of 'argsort'
</commit_message>
<xml_diff>
--- a/plot_results/roc/auc_pivot.xlsx
+++ b/plot_results/roc/auc_pivot.xlsx
@@ -37,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -50,6 +50,27 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -425,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,40 +462,45 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Classifier</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>DM-δ</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>DM-γ</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>DM-κ</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>BB</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Prob.</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Magnet</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>FS</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>RC</t>
         </is>
@@ -486,218 +512,934 @@
           <t>Ames</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>5</v>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
       </c>
       <c r="C2" t="n">
         <v>7</v>
       </c>
       <c r="D2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>BBBP</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>5</v>
+      <c r="A3" s="1" t="n"/>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>NN</t>
+        </is>
       </c>
       <c r="C3" t="n">
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G3" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I3" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Cancer</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>7</v>
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
         <v>4</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>CYP1A2</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>5</v>
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
+          <t>BBBP</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>6</v>
+      </c>
+      <c r="E6" t="n">
+        <v>7</v>
+      </c>
+      <c r="F6" t="n">
+        <v>8</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>NN</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>6</v>
+      </c>
+      <c r="F7" t="n">
+        <v>7</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" t="n">
+        <v>4</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" t="n">
+        <v>7</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6</v>
+      </c>
+      <c r="F8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>5</v>
+      </c>
+      <c r="I8" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" t="n">
+        <v>7</v>
+      </c>
+      <c r="F9" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" t="n">
+        <v>4</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>CYP1A2</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>6</v>
+      </c>
+      <c r="E10" t="n">
+        <v>7</v>
+      </c>
+      <c r="F10" t="n">
+        <v>8</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="n">
+        <v>4</v>
+      </c>
+      <c r="I10" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>NN</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>6</v>
+      </c>
+      <c r="E11" t="n">
+        <v>7</v>
+      </c>
+      <c r="F11" t="n">
+        <v>8</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>4</v>
+      </c>
+      <c r="I11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n"/>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>5</v>
+      </c>
+      <c r="D12" t="n">
+        <v>6</v>
+      </c>
+      <c r="E12" t="n">
+        <v>7</v>
+      </c>
+      <c r="F12" t="n">
+        <v>8</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>4</v>
+      </c>
+      <c r="I12" t="n">
+        <v>3</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n"/>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>6</v>
+      </c>
+      <c r="E13" t="n">
+        <v>7</v>
+      </c>
+      <c r="F13" t="n">
+        <v>8</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="n">
+        <v>4</v>
+      </c>
+      <c r="I13" t="n">
+        <v>3</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Cancer</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>7</v>
+      </c>
+      <c r="D14" t="n">
+        <v>5</v>
+      </c>
+      <c r="E14" t="n">
+        <v>6</v>
+      </c>
+      <c r="F14" t="n">
+        <v>8</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3</v>
+      </c>
+      <c r="H14" t="n">
+        <v>4</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n"/>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>NN</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>7</v>
+      </c>
+      <c r="D15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E15" t="n">
+        <v>5</v>
+      </c>
+      <c r="F15" t="n">
+        <v>8</v>
+      </c>
+      <c r="G15" t="n">
+        <v>4</v>
+      </c>
+      <c r="H15" t="n">
+        <v>2</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n"/>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>7</v>
+      </c>
+      <c r="D16" t="n">
+        <v>6</v>
+      </c>
+      <c r="E16" t="n">
+        <v>5</v>
+      </c>
+      <c r="F16" t="n">
+        <v>8</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2</v>
+      </c>
+      <c r="H16" t="n">
+        <v>4</v>
+      </c>
+      <c r="I16" t="n">
+        <v>3</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n"/>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>7</v>
+      </c>
+      <c r="D17" t="n">
+        <v>5</v>
+      </c>
+      <c r="E17" t="n">
+        <v>6</v>
+      </c>
+      <c r="F17" t="n">
+        <v>8</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3</v>
+      </c>
+      <c r="H17" t="n">
+        <v>2</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>HIV</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>5</v>
+      </c>
+      <c r="D18" t="n">
+        <v>6</v>
+      </c>
+      <c r="E18" t="n">
+        <v>8</v>
+      </c>
+      <c r="F18" t="n">
+        <v>7</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>4</v>
+      </c>
+      <c r="I18" t="n">
+        <v>3</v>
+      </c>
+      <c r="J18" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n"/>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>NN</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>6</v>
+      </c>
+      <c r="D19" t="n">
+        <v>8</v>
+      </c>
+      <c r="E19" t="n">
+        <v>7</v>
+      </c>
+      <c r="F19" t="n">
+        <v>5</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" t="n">
+        <v>4</v>
+      </c>
+      <c r="I19" t="n">
+        <v>3</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n"/>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" t="n">
+        <v>8</v>
+      </c>
+      <c r="E20" t="n">
+        <v>7</v>
+      </c>
+      <c r="F20" t="n">
+        <v>5</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" t="n">
+        <v>3</v>
+      </c>
+      <c r="I20" t="n">
+        <v>2</v>
+      </c>
+      <c r="J20" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n"/>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" t="n">
+        <v>6</v>
+      </c>
+      <c r="E21" t="n">
+        <v>7</v>
+      </c>
+      <c r="F21" t="n">
+        <v>5</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>8</v>
+      </c>
+      <c r="I21" t="n">
+        <v>3</v>
+      </c>
+      <c r="J21" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>Liver</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>8</v>
+      </c>
+      <c r="D22" t="n">
+        <v>5</v>
+      </c>
+      <c r="E22" t="n">
+        <v>4</v>
+      </c>
+      <c r="F22" t="n">
+        <v>7</v>
+      </c>
+      <c r="G22" t="n">
+        <v>3</v>
+      </c>
+      <c r="H22" t="n">
+        <v>2</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n"/>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>NN</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>7</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2</v>
+      </c>
+      <c r="E23" t="n">
+        <v>4</v>
+      </c>
+      <c r="F23" t="n">
+        <v>6</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" t="n">
+        <v>8</v>
+      </c>
+      <c r="I23" t="n">
+        <v>3</v>
+      </c>
+      <c r="J23" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n"/>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>8</v>
+      </c>
+      <c r="D24" t="n">
+        <v>6</v>
+      </c>
+      <c r="E24" t="n">
+        <v>5</v>
+      </c>
+      <c r="F24" t="n">
+        <v>7</v>
+      </c>
+      <c r="G24" t="n">
+        <v>2</v>
+      </c>
+      <c r="H24" t="n">
+        <v>4</v>
+      </c>
+      <c r="I24" t="n">
+        <v>3</v>
+      </c>
+      <c r="J24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n"/>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>7</v>
+      </c>
+      <c r="D25" t="n">
+        <v>5</v>
+      </c>
+      <c r="E25" t="n">
+        <v>6</v>
+      </c>
+      <c r="F25" t="n">
+        <v>8</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" t="n">
+        <v>2</v>
+      </c>
+      <c r="I25" t="n">
+        <v>3</v>
+      </c>
+      <c r="J25" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
           <t>hERG</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>6</v>
-      </c>
-      <c r="C6" t="n">
-        <v>7</v>
-      </c>
-      <c r="D6" t="n">
-        <v>8</v>
-      </c>
-      <c r="E6" t="n">
-        <v>5</v>
-      </c>
-      <c r="F6" t="n">
-        <v>4</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>HIV</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" t="n">
-        <v>6</v>
-      </c>
-      <c r="D7" t="n">
-        <v>7</v>
-      </c>
-      <c r="E7" t="n">
-        <v>8</v>
-      </c>
-      <c r="F7" t="n">
-        <v>4</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>3</v>
-      </c>
-      <c r="I7" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Liver</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="n">
-        <v>8</v>
-      </c>
-      <c r="D8" t="n">
-        <v>5</v>
-      </c>
-      <c r="E8" t="n">
-        <v>6</v>
-      </c>
-      <c r="F8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" t="n">
-        <v>4</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" t="n">
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>KNN</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>6</v>
+      </c>
+      <c r="D26" t="n">
+        <v>7</v>
+      </c>
+      <c r="E26" t="n">
+        <v>8</v>
+      </c>
+      <c r="F26" t="n">
+        <v>5</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" t="n">
+        <v>4</v>
+      </c>
+      <c r="I26" t="n">
+        <v>2</v>
+      </c>
+      <c r="J26" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n"/>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>NN</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D27" t="n">
+        <v>6</v>
+      </c>
+      <c r="E27" t="n">
+        <v>8</v>
+      </c>
+      <c r="F27" t="n">
+        <v>7</v>
+      </c>
+      <c r="G27" t="n">
+        <v>2</v>
+      </c>
+      <c r="H27" t="n">
+        <v>5</v>
+      </c>
+      <c r="I27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J27" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n"/>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>RF</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>6</v>
+      </c>
+      <c r="D28" t="n">
+        <v>7</v>
+      </c>
+      <c r="E28" t="n">
+        <v>8</v>
+      </c>
+      <c r="F28" t="n">
+        <v>5</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" t="n">
+        <v>4</v>
+      </c>
+      <c r="I28" t="n">
+        <v>2</v>
+      </c>
+      <c r="J28" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n"/>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>6</v>
+      </c>
+      <c r="D29" t="n">
+        <v>8</v>
+      </c>
+      <c r="E29" t="n">
+        <v>7</v>
+      </c>
+      <c r="F29" t="n">
+        <v>5</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" t="n">
+        <v>4</v>
+      </c>
+      <c r="I29" t="n">
+        <v>2</v>
+      </c>
+      <c r="J29" t="n">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A26:A29"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>